<commit_message>
Updated the files in the Output folder. Closes #3 Signed-off-by: shakirairfaan <shakirairfaan@gmail.com>
</commit_message>
<xml_diff>
--- a/StructureDefinition-lk-core-address.xlsx
+++ b/StructureDefinition-lk-core-address.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="159">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-08-14T13:12:37+05:30</t>
+    <t>2023-09-05T15:30:49+05:30</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -134,6 +134,10 @@
 </t>
   </si>
   <si>
+    <t xml:space="preserve">ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
+</t>
+  </si>
+  <si>
     <t>XAD</t>
   </si>
   <si>
@@ -212,6 +216,19 @@
     <t>LK Core MOH Area Extension</t>
   </si>
   <si>
+    <t>Address.extension:gn</t>
+  </si>
+  <si>
+    <t>gn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {http://fhir.health.gov.lk/StructureDefinition/lk-core-gn-area-ext}
+</t>
+  </si>
+  <si>
+    <t>LK Core GN Area Extension</t>
+  </si>
+  <si>
     <t>Address.use</t>
   </si>
   <si>
@@ -244,10 +261,6 @@
   </si>
   <si>
     <t>http://hl7.org/fhir/ValueSet/address-use|4.0.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-</t>
   </si>
   <si>
     <t>XAD.7</t>
@@ -780,7 +793,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AN14"/>
+  <dimension ref="A1:AN15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -928,13 +941,13 @@
         <v>38</v>
       </c>
       <c r="AJ1" t="s" s="2">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="AK1" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AL1" t="s" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AM1" t="s" s="2">
         <v>24</v>
@@ -945,10 +958,10 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" t="s" s="2">
@@ -959,7 +972,7 @@
         <v>32</v>
       </c>
       <c r="G2" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H2" t="s" s="2">
         <v>31</v>
@@ -971,13 +984,13 @@
         <v>31</v>
       </c>
       <c r="K2" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="L2" t="s" s="2">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="M2" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
@@ -1028,13 +1041,13 @@
         <v>31</v>
       </c>
       <c r="AF2" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AG2" t="s" s="2">
         <v>32</v>
       </c>
       <c r="AH2" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AI2" t="s" s="2">
         <v>31</v>
@@ -1046,7 +1059,7 @@
         <v>31</v>
       </c>
       <c r="AL2" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AM2" t="s" s="2">
         <v>31</v>
@@ -1057,14 +1070,14 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" t="s" s="2">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" t="s" s="2">
@@ -1083,16 +1096,16 @@
         <v>31</v>
       </c>
       <c r="K3" t="s" s="2">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L3" t="s" s="2">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M3" t="s" s="2">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="N3" t="s" s="2">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="O3" s="2"/>
       <c r="P3" t="s" s="2">
@@ -1130,19 +1143,19 @@
         <v>31</v>
       </c>
       <c r="AB3" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AC3" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AD3" t="s" s="2">
         <v>31</v>
       </c>
       <c r="AE3" t="s" s="2">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AF3" t="s" s="2">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AG3" t="s" s="2">
         <v>32</v>
@@ -1154,13 +1167,13 @@
         <v>31</v>
       </c>
       <c r="AJ3" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AK3" t="s" s="2">
         <v>31</v>
       </c>
       <c r="AL3" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AM3" t="s" s="2">
         <v>31</v>
@@ -1171,13 +1184,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C4" t="s" s="2">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D4" t="s" s="2">
         <v>31</v>
@@ -1187,7 +1200,7 @@
         <v>32</v>
       </c>
       <c r="G4" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H4" t="s" s="2">
         <v>31</v>
@@ -1199,13 +1212,13 @@
         <v>31</v>
       </c>
       <c r="K4" t="s" s="2">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L4" t="s" s="2">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="M4" t="s" s="2">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
@@ -1256,7 +1269,7 @@
         <v>31</v>
       </c>
       <c r="AF4" t="s" s="2">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AG4" t="s" s="2">
         <v>32</v>
@@ -1268,7 +1281,7 @@
         <v>31</v>
       </c>
       <c r="AJ4" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AK4" t="s" s="2">
         <v>31</v>
@@ -1285,12 +1298,14 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>63</v>
-      </c>
-      <c r="C5" s="2"/>
+        <v>49</v>
+      </c>
+      <c r="C5" t="s" s="2">
+        <v>65</v>
+      </c>
       <c r="D5" t="s" s="2">
         <v>31</v>
       </c>
@@ -1299,32 +1314,28 @@
         <v>32</v>
       </c>
       <c r="G5" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H5" t="s" s="2">
         <v>31</v>
       </c>
       <c r="I5" t="s" s="2">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="J5" t="s" s="2">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="K5" t="s" s="2">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L5" t="s" s="2">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="M5" t="s" s="2">
         <v>67</v>
       </c>
-      <c r="N5" t="s" s="2">
-        <v>68</v>
-      </c>
-      <c r="O5" t="s" s="2">
-        <v>69</v>
-      </c>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
       <c r="P5" t="s" s="2">
         <v>31</v>
       </c>
@@ -1336,7 +1347,7 @@
         <v>31</v>
       </c>
       <c r="T5" t="s" s="2">
-        <v>70</v>
+        <v>31</v>
       </c>
       <c r="U5" t="s" s="2">
         <v>31</v>
@@ -1348,13 +1359,13 @@
         <v>31</v>
       </c>
       <c r="X5" t="s" s="2">
-        <v>71</v>
+        <v>31</v>
       </c>
       <c r="Y5" t="s" s="2">
-        <v>72</v>
+        <v>31</v>
       </c>
       <c r="Z5" t="s" s="2">
-        <v>73</v>
+        <v>31</v>
       </c>
       <c r="AA5" t="s" s="2">
         <v>31</v>
@@ -1372,28 +1383,28 @@
         <v>31</v>
       </c>
       <c r="AF5" t="s" s="2">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="AG5" t="s" s="2">
         <v>32</v>
       </c>
       <c r="AH5" t="s" s="2">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="AI5" t="s" s="2">
         <v>31</v>
       </c>
       <c r="AJ5" t="s" s="2">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="AK5" t="s" s="2">
-        <v>75</v>
+        <v>31</v>
       </c>
       <c r="AL5" t="s" s="2">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="AM5" t="s" s="2">
-        <v>77</v>
+        <v>31</v>
       </c>
       <c r="AN5" t="s" s="2">
         <v>31</v>
@@ -1401,10 +1412,10 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" t="s" s="2">
@@ -1415,30 +1426,32 @@
         <v>32</v>
       </c>
       <c r="G6" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H6" t="s" s="2">
         <v>31</v>
       </c>
       <c r="I6" t="s" s="2">
-        <v>31</v>
+        <v>69</v>
       </c>
       <c r="J6" t="s" s="2">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="K6" t="s" s="2">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="L6" t="s" s="2">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="M6" t="s" s="2">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="N6" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="O6" s="2"/>
+        <v>73</v>
+      </c>
+      <c r="O6" t="s" s="2">
+        <v>74</v>
+      </c>
       <c r="P6" t="s" s="2">
         <v>31</v>
       </c>
@@ -1450,7 +1463,7 @@
         <v>31</v>
       </c>
       <c r="T6" t="s" s="2">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="U6" t="s" s="2">
         <v>31</v>
@@ -1462,13 +1475,13 @@
         <v>31</v>
       </c>
       <c r="X6" t="s" s="2">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="Y6" t="s" s="2">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="Z6" t="s" s="2">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="AA6" t="s" s="2">
         <v>31</v>
@@ -1486,39 +1499,39 @@
         <v>31</v>
       </c>
       <c r="AF6" t="s" s="2">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="AG6" t="s" s="2">
         <v>32</v>
       </c>
       <c r="AH6" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AI6" t="s" s="2">
         <v>31</v>
       </c>
       <c r="AJ6" t="s" s="2">
-        <v>74</v>
+        <v>39</v>
       </c>
       <c r="AK6" t="s" s="2">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="AL6" t="s" s="2">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="AM6" t="s" s="2">
-        <v>31</v>
+        <v>81</v>
       </c>
       <c r="AN6" t="s" s="2">
-        <v>86</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" t="s" s="2">
@@ -1529,7 +1542,7 @@
         <v>32</v>
       </c>
       <c r="G7" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H7" t="s" s="2">
         <v>31</v>
@@ -1538,23 +1551,21 @@
         <v>31</v>
       </c>
       <c r="J7" t="s" s="2">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="K7" t="s" s="2">
-        <v>43</v>
+        <v>70</v>
       </c>
       <c r="L7" t="s" s="2">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="M7" t="s" s="2">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="N7" t="s" s="2">
-        <v>90</v>
-      </c>
-      <c r="O7" t="s" s="2">
-        <v>91</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="O7" s="2"/>
       <c r="P7" t="s" s="2">
         <v>31</v>
       </c>
@@ -1566,7 +1577,7 @@
         <v>31</v>
       </c>
       <c r="T7" t="s" s="2">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="U7" t="s" s="2">
         <v>31</v>
@@ -1578,13 +1589,13 @@
         <v>31</v>
       </c>
       <c r="X7" t="s" s="2">
-        <v>31</v>
+        <v>76</v>
       </c>
       <c r="Y7" t="s" s="2">
-        <v>31</v>
+        <v>87</v>
       </c>
       <c r="Z7" t="s" s="2">
-        <v>31</v>
+        <v>88</v>
       </c>
       <c r="AA7" t="s" s="2">
         <v>31</v>
@@ -1602,39 +1613,39 @@
         <v>31</v>
       </c>
       <c r="AF7" t="s" s="2">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="AG7" t="s" s="2">
         <v>32</v>
       </c>
       <c r="AH7" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AI7" t="s" s="2">
         <v>31</v>
       </c>
       <c r="AJ7" t="s" s="2">
-        <v>74</v>
+        <v>39</v>
       </c>
       <c r="AK7" t="s" s="2">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="AL7" t="s" s="2">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="AM7" t="s" s="2">
         <v>31</v>
       </c>
       <c r="AN7" t="s" s="2">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" t="s" s="2">
@@ -1645,7 +1656,7 @@
         <v>32</v>
       </c>
       <c r="G8" t="s" s="2">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="H8" t="s" s="2">
         <v>31</v>
@@ -1654,19 +1665,23 @@
         <v>31</v>
       </c>
       <c r="J8" t="s" s="2">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="K8" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="L8" t="s" s="2">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="M8" t="s" s="2">
-        <v>98</v>
-      </c>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
+        <v>93</v>
+      </c>
+      <c r="N8" t="s" s="2">
+        <v>94</v>
+      </c>
+      <c r="O8" t="s" s="2">
+        <v>95</v>
+      </c>
       <c r="P8" t="s" s="2">
         <v>31</v>
       </c>
@@ -1678,86 +1693,86 @@
         <v>31</v>
       </c>
       <c r="T8" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="U8" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="V8" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="W8" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="X8" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="Y8" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="Z8" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="AA8" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="AB8" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="AC8" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="AD8" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="AE8" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="AF8" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="AG8" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="AH8" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AI8" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="AJ8" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AK8" t="s" s="2">
+        <v>97</v>
+      </c>
+      <c r="AL8" t="s" s="2">
+        <v>98</v>
+      </c>
+      <c r="AM8" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="AN8" t="s" s="2">
         <v>99</v>
-      </c>
-      <c r="U8" t="s" s="2">
-        <v>31</v>
-      </c>
-      <c r="V8" t="s" s="2">
-        <v>31</v>
-      </c>
-      <c r="W8" t="s" s="2">
-        <v>31</v>
-      </c>
-      <c r="X8" t="s" s="2">
-        <v>31</v>
-      </c>
-      <c r="Y8" t="s" s="2">
-        <v>31</v>
-      </c>
-      <c r="Z8" t="s" s="2">
-        <v>31</v>
-      </c>
-      <c r="AA8" t="s" s="2">
-        <v>31</v>
-      </c>
-      <c r="AB8" t="s" s="2">
-        <v>31</v>
-      </c>
-      <c r="AC8" t="s" s="2">
-        <v>31</v>
-      </c>
-      <c r="AD8" t="s" s="2">
-        <v>31</v>
-      </c>
-      <c r="AE8" t="s" s="2">
-        <v>31</v>
-      </c>
-      <c r="AF8" t="s" s="2">
-        <v>96</v>
-      </c>
-      <c r="AG8" t="s" s="2">
-        <v>32</v>
-      </c>
-      <c r="AH8" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="AI8" t="s" s="2">
-        <v>31</v>
-      </c>
-      <c r="AJ8" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AK8" t="s" s="2">
-        <v>100</v>
-      </c>
-      <c r="AL8" t="s" s="2">
-        <v>101</v>
-      </c>
-      <c r="AM8" t="s" s="2">
-        <v>102</v>
-      </c>
-      <c r="AN8" t="s" s="2">
-        <v>103</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B9" t="s" s="2">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" t="s" s="2">
-        <v>105</v>
+        <v>31</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" t="s" s="2">
         <v>32</v>
       </c>
       <c r="G9" t="s" s="2">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="H9" t="s" s="2">
         <v>31</v>
@@ -1766,16 +1781,16 @@
         <v>31</v>
       </c>
       <c r="J9" t="s" s="2">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="K9" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="L9" t="s" s="2">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="M9" t="s" s="2">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
@@ -1790,7 +1805,7 @@
         <v>31</v>
       </c>
       <c r="T9" t="s" s="2">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="U9" t="s" s="2">
         <v>31</v>
@@ -1826,50 +1841,50 @@
         <v>31</v>
       </c>
       <c r="AF9" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="AG9" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="AH9" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="AI9" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="AJ9" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AK9" t="s" s="2">
         <v>104</v>
       </c>
-      <c r="AG9" t="s" s="2">
-        <v>32</v>
-      </c>
-      <c r="AH9" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AI9" t="s" s="2">
-        <v>31</v>
-      </c>
-      <c r="AJ9" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AK9" t="s" s="2">
-        <v>109</v>
-      </c>
       <c r="AL9" t="s" s="2">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="AM9" t="s" s="2">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="AN9" t="s" s="2">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" t="s" s="2">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" t="s" s="2">
         <v>32</v>
       </c>
       <c r="G10" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H10" t="s" s="2">
         <v>31</v>
@@ -1878,20 +1893,18 @@
         <v>31</v>
       </c>
       <c r="J10" t="s" s="2">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="K10" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="L10" t="s" s="2">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="M10" t="s" s="2">
-        <v>116</v>
-      </c>
-      <c r="N10" t="s" s="2">
-        <v>117</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="N10" s="2"/>
       <c r="O10" s="2"/>
       <c r="P10" t="s" s="2">
         <v>31</v>
@@ -1904,7 +1917,7 @@
         <v>31</v>
       </c>
       <c r="T10" t="s" s="2">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="U10" t="s" s="2">
         <v>31</v>
@@ -1940,50 +1953,50 @@
         <v>31</v>
       </c>
       <c r="AF10" t="s" s="2">
+        <v>108</v>
+      </c>
+      <c r="AG10" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="AH10" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AI10" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="AJ10" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AK10" t="s" s="2">
         <v>113</v>
       </c>
-      <c r="AG10" t="s" s="2">
-        <v>32</v>
-      </c>
-      <c r="AH10" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AI10" t="s" s="2">
-        <v>31</v>
-      </c>
-      <c r="AJ10" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AK10" t="s" s="2">
-        <v>119</v>
-      </c>
       <c r="AL10" t="s" s="2">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="AM10" t="s" s="2">
-        <v>31</v>
+        <v>115</v>
       </c>
       <c r="AN10" t="s" s="2">
-        <v>31</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" t="s" s="2">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" t="s" s="2">
         <v>32</v>
       </c>
       <c r="G11" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H11" t="s" s="2">
         <v>31</v>
@@ -1992,18 +2005,20 @@
         <v>31</v>
       </c>
       <c r="J11" t="s" s="2">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="K11" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="L11" t="s" s="2">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="M11" t="s" s="2">
-        <v>124</v>
-      </c>
-      <c r="N11" s="2"/>
+        <v>120</v>
+      </c>
+      <c r="N11" t="s" s="2">
+        <v>121</v>
+      </c>
       <c r="O11" s="2"/>
       <c r="P11" t="s" s="2">
         <v>31</v>
@@ -2016,7 +2031,7 @@
         <v>31</v>
       </c>
       <c r="T11" t="s" s="2">
-        <v>31</v>
+        <v>122</v>
       </c>
       <c r="U11" t="s" s="2">
         <v>31</v>
@@ -2052,50 +2067,50 @@
         <v>31</v>
       </c>
       <c r="AF11" t="s" s="2">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="AG11" t="s" s="2">
         <v>32</v>
       </c>
       <c r="AH11" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AI11" t="s" s="2">
         <v>31</v>
       </c>
       <c r="AJ11" t="s" s="2">
-        <v>74</v>
+        <v>39</v>
       </c>
       <c r="AK11" t="s" s="2">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="AL11" t="s" s="2">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="AM11" t="s" s="2">
-        <v>127</v>
+        <v>31</v>
       </c>
       <c r="AN11" t="s" s="2">
-        <v>128</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" t="s" s="2">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" t="s" s="2">
         <v>32</v>
       </c>
       <c r="G12" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H12" t="s" s="2">
         <v>31</v>
@@ -2104,16 +2119,16 @@
         <v>31</v>
       </c>
       <c r="J12" t="s" s="2">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="K12" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="L12" t="s" s="2">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="M12" t="s" s="2">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
@@ -2128,7 +2143,7 @@
         <v>31</v>
       </c>
       <c r="T12" t="s" s="2">
-        <v>133</v>
+        <v>31</v>
       </c>
       <c r="U12" t="s" s="2">
         <v>31</v>
@@ -2164,50 +2179,50 @@
         <v>31</v>
       </c>
       <c r="AF12" t="s" s="2">
+        <v>125</v>
+      </c>
+      <c r="AG12" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="AH12" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AI12" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="AJ12" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AK12" t="s" s="2">
         <v>129</v>
       </c>
-      <c r="AG12" t="s" s="2">
-        <v>32</v>
-      </c>
-      <c r="AH12" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AI12" t="s" s="2">
-        <v>31</v>
-      </c>
-      <c r="AJ12" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AK12" t="s" s="2">
-        <v>134</v>
-      </c>
       <c r="AL12" t="s" s="2">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="AM12" t="s" s="2">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="AN12" t="s" s="2">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" t="s" s="2">
-        <v>31</v>
+        <v>134</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" t="s" s="2">
         <v>32</v>
       </c>
       <c r="G13" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H13" t="s" s="2">
         <v>31</v>
@@ -2216,20 +2231,18 @@
         <v>31</v>
       </c>
       <c r="J13" t="s" s="2">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="K13" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="L13" t="s" s="2">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="M13" t="s" s="2">
-        <v>140</v>
-      </c>
-      <c r="N13" t="s" s="2">
-        <v>141</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="N13" s="2"/>
       <c r="O13" s="2"/>
       <c r="P13" t="s" s="2">
         <v>31</v>
@@ -2242,7 +2255,7 @@
         <v>31</v>
       </c>
       <c r="T13" t="s" s="2">
-        <v>31</v>
+        <v>137</v>
       </c>
       <c r="U13" t="s" s="2">
         <v>31</v>
@@ -2278,39 +2291,39 @@
         <v>31</v>
       </c>
       <c r="AF13" t="s" s="2">
+        <v>133</v>
+      </c>
+      <c r="AG13" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="AH13" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AI13" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="AJ13" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AK13" t="s" s="2">
         <v>138</v>
       </c>
-      <c r="AG13" t="s" s="2">
-        <v>32</v>
-      </c>
-      <c r="AH13" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AI13" t="s" s="2">
-        <v>31</v>
-      </c>
-      <c r="AJ13" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AK13" t="s" s="2">
-        <v>142</v>
-      </c>
       <c r="AL13" t="s" s="2">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="AM13" t="s" s="2">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="AN13" t="s" s="2">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B14" t="s" s="2">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" t="s" s="2">
@@ -2321,7 +2334,7 @@
         <v>32</v>
       </c>
       <c r="G14" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H14" t="s" s="2">
         <v>31</v>
@@ -2330,21 +2343,21 @@
         <v>31</v>
       </c>
       <c r="J14" t="s" s="2">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="K14" t="s" s="2">
-        <v>147</v>
+        <v>44</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="M14" t="s" s="2">
-        <v>149</v>
-      </c>
-      <c r="N14" s="2"/>
-      <c r="O14" t="s" s="2">
-        <v>150</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="N14" t="s" s="2">
+        <v>145</v>
+      </c>
+      <c r="O14" s="2"/>
       <c r="P14" t="s" s="2">
         <v>31</v>
       </c>
@@ -2356,66 +2369,180 @@
         <v>31</v>
       </c>
       <c r="T14" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="U14" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="V14" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="W14" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="X14" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="Y14" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="Z14" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="AA14" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="AB14" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="AC14" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="AD14" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="AE14" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="AF14" t="s" s="2">
+        <v>142</v>
+      </c>
+      <c r="AG14" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="AH14" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AI14" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="AJ14" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AK14" t="s" s="2">
+        <v>146</v>
+      </c>
+      <c r="AL14" t="s" s="2">
+        <v>147</v>
+      </c>
+      <c r="AM14" t="s" s="2">
+        <v>148</v>
+      </c>
+      <c r="AN14" t="s" s="2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="2">
+        <v>150</v>
+      </c>
+      <c r="B15" t="s" s="2">
+        <v>150</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="G15" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="H15" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="I15" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="J15" t="s" s="2">
+        <v>69</v>
+      </c>
+      <c r="K15" t="s" s="2">
         <v>151</v>
       </c>
-      <c r="U14" t="s" s="2">
-        <v>31</v>
-      </c>
-      <c r="V14" t="s" s="2">
-        <v>31</v>
-      </c>
-      <c r="W14" t="s" s="2">
-        <v>31</v>
-      </c>
-      <c r="X14" t="s" s="2">
-        <v>31</v>
-      </c>
-      <c r="Y14" t="s" s="2">
-        <v>31</v>
-      </c>
-      <c r="Z14" t="s" s="2">
-        <v>31</v>
-      </c>
-      <c r="AA14" t="s" s="2">
-        <v>31</v>
-      </c>
-      <c r="AB14" t="s" s="2">
-        <v>31</v>
-      </c>
-      <c r="AC14" t="s" s="2">
-        <v>31</v>
-      </c>
-      <c r="AD14" t="s" s="2">
-        <v>31</v>
-      </c>
-      <c r="AE14" t="s" s="2">
-        <v>31</v>
-      </c>
-      <c r="AF14" t="s" s="2">
-        <v>146</v>
-      </c>
-      <c r="AG14" t="s" s="2">
-        <v>32</v>
-      </c>
-      <c r="AH14" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AI14" t="s" s="2">
-        <v>31</v>
-      </c>
-      <c r="AJ14" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AK14" t="s" s="2">
+      <c r="L15" t="s" s="2">
         <v>152</v>
       </c>
-      <c r="AL14" t="s" s="2">
+      <c r="M15" t="s" s="2">
         <v>153</v>
       </c>
-      <c r="AM14" t="s" s="2">
+      <c r="N15" s="2"/>
+      <c r="O15" t="s" s="2">
         <v>154</v>
       </c>
-      <c r="AN14" t="s" s="2">
+      <c r="P15" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="Q15" s="2"/>
+      <c r="R15" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="S15" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="T15" t="s" s="2">
+        <v>155</v>
+      </c>
+      <c r="U15" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="V15" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="W15" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="X15" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="Y15" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="Z15" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="AA15" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="AB15" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="AC15" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="AD15" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="AE15" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="AF15" t="s" s="2">
+        <v>150</v>
+      </c>
+      <c r="AG15" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="AH15" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AI15" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="AJ15" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AK15" t="s" s="2">
+        <v>156</v>
+      </c>
+      <c r="AL15" t="s" s="2">
+        <v>157</v>
+      </c>
+      <c r="AM15" t="s" s="2">
+        <v>158</v>
+      </c>
+      <c r="AN15" t="s" s="2">
         <v>31</v>
       </c>
     </row>

</xml_diff>